<commit_message>
Add analyse des entrées
</commit_message>
<xml_diff>
--- a/TableVerite.xlsx
+++ b/TableVerite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca4be0296f990297/Documents/Etudes/HEIG/2eme/Semestre3/SYL/Laboratoires/SYL_Labo4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07E1F149-5369-4708-B0BF-779967282CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{07E1F149-5369-4708-B0BF-779967282CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA6A55D0-EA76-449F-94EB-A34DD4D16C68}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7EEE2296-4C3C-4797-896E-A9F0270D27D2}"/>
   </bookViews>
@@ -218,12 +218,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FBBB43-88E7-4F1B-9133-23BBDCBCFDED}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,54 +551,55 @@
     <col min="3" max="5" width="8.88671875" style="1"/>
     <col min="6" max="11" width="10.109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="3"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>